<commit_message>
ajustando codigo e procurando soluções por meio de XML
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE_Joas.xlsx
+++ b/testes/resultado_inferência_NGE_Joas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA1D3D1-B33E-F04E-8A60-CAE122B4C479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358B311C-149D-CF40-B8C1-3FB656815463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33980" yWindow="2660" windowWidth="23360" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38220" yWindow="460" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inferencia por IA" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -89,14 +89,17 @@
     <t>RMSE Editorar</t>
   </si>
   <si>
-    <t>Modelo 1</t>
+    <t>Modelo 3 - log</t>
+  </si>
+  <si>
+    <t>Modelo 2 - Reg Linear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +111,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -222,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -259,6 +269,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,22 +576,30 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5" customWidth="1"/>
-    <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" customWidth="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -621,15 +641,17 @@
         <v>11</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>16</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="10" t="s">
-        <v>13</v>
+      <c r="R2" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -670,11 +692,15 @@
         <v>48</v>
       </c>
       <c r="M3">
-        <v>60.614479129388329</v>
-      </c>
-      <c r="P3" s="15"/>
+        <v>55.680476331125107</v>
+      </c>
+      <c r="N3" s="20">
+        <v>44</v>
+      </c>
+      <c r="O3" s="15"/>
+      <c r="P3" s="11"/>
       <c r="Q3" s="8"/>
-      <c r="R3" s="11"/>
+      <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -714,20 +740,25 @@
         <v>48</v>
       </c>
       <c r="M4" s="3">
-        <v>45.227512219875841</v>
-      </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="17">
+        <v>41.756478138640432</v>
+      </c>
+      <c r="N4" s="21">
+        <v>44</v>
+      </c>
+      <c r="O4" s="17">
         <v>38</v>
       </c>
+      <c r="P4" s="11">
+        <f>O4-L4</f>
+        <v>-10</v>
+      </c>
       <c r="Q4" s="8">
-        <f>P4-M4</f>
-        <v>-7.227512219875841</v>
-      </c>
-      <c r="R4" s="11">
-        <f>P4-L4</f>
-        <v>-10</v>
+        <f>O4-M4</f>
+        <v>-3.756478138640432</v>
+      </c>
+      <c r="R4" s="8">
+        <f>N4-O4</f>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -768,20 +799,25 @@
         <v>98</v>
       </c>
       <c r="M5" s="3">
-        <v>90.361287831037259</v>
-      </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="17">
+        <v>84.929670372295817</v>
+      </c>
+      <c r="N5" s="21">
+        <v>46</v>
+      </c>
+      <c r="O5" s="17">
         <v>66</v>
       </c>
+      <c r="P5" s="11">
+        <f>O5-L5</f>
+        <v>-32</v>
+      </c>
       <c r="Q5" s="8">
-        <f>P5-M5</f>
-        <v>-24.361287831037259</v>
-      </c>
-      <c r="R5" s="11">
-        <f>P5-L5</f>
-        <v>-32</v>
+        <f>O5-M5</f>
+        <v>-18.929670372295817</v>
+      </c>
+      <c r="R5" s="8">
+        <f t="shared" ref="R5:R6" si="0">N5-O5</f>
+        <v>-20</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -822,20 +858,25 @@
         <v>48</v>
       </c>
       <c r="M6" s="3">
-        <v>41.129761152837773</v>
-      </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="17">
+        <v>37.825875345796227</v>
+      </c>
+      <c r="N6" s="21">
         <v>36</v>
       </c>
+      <c r="O6" s="17">
+        <v>36</v>
+      </c>
+      <c r="P6" s="11">
+        <f>O6-L6</f>
+        <v>-12</v>
+      </c>
       <c r="Q6" s="8">
-        <f>P6-M6</f>
-        <v>-5.1297611528377729</v>
-      </c>
-      <c r="R6" s="11">
-        <f>P6-L6</f>
-        <v>-12</v>
+        <f>O6-M6</f>
+        <v>-1.8258753457962271</v>
+      </c>
+      <c r="R6" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -876,11 +917,15 @@
         <v>46</v>
       </c>
       <c r="M7">
-        <v>38.957017944117482</v>
-      </c>
-      <c r="P7" s="15"/>
+        <v>35.751889036750981</v>
+      </c>
+      <c r="N7" s="20">
+        <v>44</v>
+      </c>
+      <c r="O7" s="15"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="11"/>
+      <c r="R7" s="8"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -920,11 +965,15 @@
         <v>46</v>
       </c>
       <c r="M8">
-        <v>38.103939363613748</v>
-      </c>
-      <c r="P8" s="15"/>
+        <v>34.905428976361989</v>
+      </c>
+      <c r="N8" s="20">
+        <v>44</v>
+      </c>
+      <c r="O8" s="15"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="11"/>
+      <c r="R8" s="8"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -964,11 +1013,15 @@
         <v>46</v>
       </c>
       <c r="M9">
-        <v>36.216062147929527</v>
-      </c>
-      <c r="P9" s="15"/>
+        <v>33.078834354332727</v>
+      </c>
+      <c r="N9" s="20">
+        <v>44</v>
+      </c>
+      <c r="O9" s="15"/>
+      <c r="P9" s="11"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="11"/>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1008,11 +1061,15 @@
         <v>198</v>
       </c>
       <c r="M10">
-        <v>184.31591289508</v>
-      </c>
-      <c r="P10" s="15"/>
+        <v>173.98223948728511</v>
+      </c>
+      <c r="N10" s="20">
+        <v>296</v>
+      </c>
+      <c r="O10" s="15"/>
+      <c r="P10" s="11"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="11"/>
+      <c r="R10" s="8"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1052,11 +1109,15 @@
         <v>110</v>
       </c>
       <c r="M11">
-        <v>97.290163094152632</v>
-      </c>
-      <c r="P11" s="15"/>
+        <v>91.539508452843435</v>
+      </c>
+      <c r="N11" s="20">
+        <v>44</v>
+      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" s="11"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="11"/>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -1096,20 +1157,25 @@
         <v>68</v>
       </c>
       <c r="M12" s="3">
-        <v>64.700145597353583</v>
-      </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="17">
+        <v>59.626571692041168</v>
+      </c>
+      <c r="N12" s="21">
+        <v>44</v>
+      </c>
+      <c r="O12" s="17">
         <v>48</v>
       </c>
+      <c r="P12" s="11">
+        <f>O12-L12</f>
+        <v>-20</v>
+      </c>
       <c r="Q12" s="8">
-        <f>P12-M12</f>
-        <v>-16.700145597353583</v>
-      </c>
-      <c r="R12" s="11">
-        <f>P12-L12</f>
-        <v>-20</v>
+        <f>O12-M12</f>
+        <v>-11.626571692041168</v>
+      </c>
+      <c r="R12" s="8">
+        <f t="shared" ref="R12:R17" si="1">N12-O12</f>
+        <v>-4</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1150,11 +1216,15 @@
         <v>75</v>
       </c>
       <c r="M13">
-        <v>72.164488122104331</v>
-      </c>
-      <c r="P13" s="15"/>
+        <v>67.174074696381723</v>
+      </c>
+      <c r="N13" s="20">
+        <v>44</v>
+      </c>
+      <c r="O13" s="15"/>
+      <c r="P13" s="11"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="11"/>
+      <c r="R13" s="8"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -1194,20 +1264,25 @@
         <v>70</v>
       </c>
       <c r="M14" s="3">
-        <v>69.072285221746313</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="17">
+        <v>64.088337109654304</v>
+      </c>
+      <c r="N14" s="21">
+        <v>44</v>
+      </c>
+      <c r="O14" s="17">
         <v>54</v>
       </c>
+      <c r="P14" s="11">
+        <f>O14-L14</f>
+        <v>-16</v>
+      </c>
       <c r="Q14" s="8">
-        <f>P14-M14</f>
-        <v>-15.072285221746313</v>
-      </c>
-      <c r="R14" s="11">
-        <f>P14-L14</f>
-        <v>-16</v>
+        <f>O14-M14</f>
+        <v>-10.088337109654304</v>
+      </c>
+      <c r="R14" s="8">
+        <f t="shared" si="1"/>
+        <v>-10</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1248,20 +1323,25 @@
         <v>114</v>
       </c>
       <c r="M15" s="3">
-        <v>117.6735860749812</v>
-      </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="17">
+        <v>109.9056922983319</v>
+      </c>
+      <c r="N15" s="21">
+        <v>212</v>
+      </c>
+      <c r="O15" s="17">
         <v>76</v>
       </c>
+      <c r="P15" s="11">
+        <f>O15-L15</f>
+        <v>-38</v>
+      </c>
       <c r="Q15" s="8">
-        <f>P15-M15</f>
-        <v>-41.673586074981202</v>
-      </c>
-      <c r="R15" s="11">
-        <f>P15-L15</f>
-        <v>-38</v>
+        <f>O15-M15</f>
+        <v>-33.9056922983319</v>
+      </c>
+      <c r="R15" s="8">
+        <f t="shared" si="1"/>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1302,20 +1382,25 @@
         <v>460</v>
       </c>
       <c r="M16" s="3">
-        <v>496.38130347050412</v>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="17">
+        <v>473.38039538904297</v>
+      </c>
+      <c r="N16" s="21">
+        <v>340</v>
+      </c>
+      <c r="O16" s="17">
         <v>414</v>
       </c>
+      <c r="P16" s="11">
+        <f>O16-L16</f>
+        <v>-46</v>
+      </c>
       <c r="Q16" s="8">
-        <f>P16-M16</f>
-        <v>-82.381303470504122</v>
-      </c>
-      <c r="R16" s="11">
-        <f>P16-L16</f>
-        <v>-46</v>
+        <f>O16-M16</f>
+        <v>-59.380395389042974</v>
+      </c>
+      <c r="R16" s="8">
+        <f t="shared" si="1"/>
+        <v>-74</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -1356,20 +1441,25 @@
         <v>420</v>
       </c>
       <c r="M17" s="3">
-        <v>441.12890291467102</v>
-      </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="17">
+        <v>420.38506339881877</v>
+      </c>
+      <c r="N17" s="21">
+        <v>296</v>
+      </c>
+      <c r="O17" s="17">
         <v>398</v>
       </c>
+      <c r="P17" s="11">
+        <f>O17-L17</f>
+        <v>-22</v>
+      </c>
       <c r="Q17" s="8">
-        <f>P17-M17</f>
-        <v>-43.128902914671016</v>
-      </c>
-      <c r="R17" s="11">
-        <f>P17-L17</f>
-        <v>-22</v>
+        <f>O17-M17</f>
+        <v>-22.385063398818772</v>
+      </c>
+      <c r="R17" s="8">
+        <f t="shared" si="1"/>
+        <v>-102</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1410,9 +1500,13 @@
         <v>48</v>
       </c>
       <c r="M18">
-        <v>45.358025866913707</v>
-      </c>
-      <c r="P18" s="15"/>
+        <v>41.900994858328531</v>
+      </c>
+      <c r="N18" s="20">
+        <v>44</v>
+      </c>
+      <c r="O18" s="15"/>
+      <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
     </row>
@@ -1453,31 +1547,41 @@
       <c r="L19" s="6">
         <v>48</v>
       </c>
-      <c r="M19" s="6">
-        <v>43.542796977152143</v>
-      </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="16"/>
+      <c r="M19">
+        <v>39.768322133434268</v>
+      </c>
+      <c r="N19" s="20">
+        <v>44</v>
+      </c>
+      <c r="O19" s="16"/>
+      <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P20" t="s">
+      <c r="O20" t="s">
         <v>14</v>
+      </c>
+      <c r="P20">
+        <f>SUMSQ(P3:P19)</f>
+        <v>5968</v>
       </c>
       <c r="Q20">
         <f>SUMSQ(Q4:Q17)</f>
-        <v>11561.561576410022</v>
+        <v>5789.4474742938201</v>
       </c>
       <c r="R20">
-        <f>SUMSQ(R3:R19)</f>
-        <v>5968</v>
+        <f>SUMSQ(R4:R17)</f>
+        <v>34928</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P21" t="s">
+      <c r="O21" t="s">
         <v>15</v>
+      </c>
+      <c r="P21">
+        <f>COUNT(O3:O19)</f>
+        <v>8</v>
       </c>
       <c r="Q21">
         <f>COUNT(P3:P19)</f>
@@ -1489,21 +1593,28 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P23" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="Q23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R23" s="12" t="s">
-        <v>18</v>
+      <c r="R23" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P24" s="13">
+        <f>SQRT(P20/P21)</f>
+        <v>27.313000567495326</v>
+      </c>
       <c r="Q24" s="5">
         <f>SQRT(Q20/Q21)</f>
-        <v>38.015723024181099</v>
-      </c>
-      <c r="R24" s="13">
+        <v>26.901318448855392</v>
+      </c>
+      <c r="R24" s="5">
         <f>SQRT(R20/R21)</f>
-        <v>27.313000567495326</v>
+        <v>66.075714146727165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção codigo para colocar pagina word via XLM e colocando arquivo word correto, pois estavam as paginas de apresentação apenas. Isso contaminou o treinamento. RESULTADO MELHORIA SIGNIFICATIVA NO MODELO
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE_Joas.xlsx
+++ b/testes/resultado_inferência_NGE_Joas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162BED46-D19F-E347-8877-0D9E9B759E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14CC622-AC90-1540-B69A-AD7938835F6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38220" yWindow="460" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -111,6 +111,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -573,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -692,7 +693,7 @@
         <v>48</v>
       </c>
       <c r="M3">
-        <v>55.680476331125107</v>
+        <v>54.605536396961817</v>
       </c>
       <c r="N3" s="20">
         <v>44</v>
@@ -739,8 +740,8 @@
       <c r="L4" s="3">
         <v>48</v>
       </c>
-      <c r="M4" s="3">
-        <v>41.756478138640432</v>
+      <c r="M4">
+        <v>41.856676411395242</v>
       </c>
       <c r="N4" s="21">
         <v>44</v>
@@ -754,7 +755,7 @@
       </c>
       <c r="Q4" s="8">
         <f>O4-M4</f>
-        <v>-3.756478138640432</v>
+        <v>-3.8566764113952416</v>
       </c>
       <c r="R4" s="8">
         <f>N4-O4</f>
@@ -798,8 +799,8 @@
       <c r="L5" s="3">
         <v>98</v>
       </c>
-      <c r="M5" s="3">
-        <v>84.929670372295817</v>
+      <c r="M5">
+        <v>87.577477027577629</v>
       </c>
       <c r="N5" s="21">
         <v>46</v>
@@ -813,7 +814,7 @@
       </c>
       <c r="Q5" s="8">
         <f>O5-M5</f>
-        <v>-18.929670372295817</v>
+        <v>-21.577477027577629</v>
       </c>
       <c r="R5" s="8">
         <f t="shared" ref="R5:R6" si="0">N5-O5</f>
@@ -857,8 +858,8 @@
       <c r="L6" s="3">
         <v>48</v>
       </c>
-      <c r="M6" s="3">
-        <v>37.825875345796227</v>
+      <c r="M6">
+        <v>37.377088243648622</v>
       </c>
       <c r="N6" s="21">
         <v>36</v>
@@ -872,7 +873,7 @@
       </c>
       <c r="Q6" s="8">
         <f>O6-M6</f>
-        <v>-1.8258753457962271</v>
+        <v>-1.3770882436486218</v>
       </c>
       <c r="R6" s="8">
         <f t="shared" si="0"/>
@@ -917,7 +918,7 @@
         <v>46</v>
       </c>
       <c r="M7">
-        <v>35.751889036750981</v>
+        <v>35.401481552743753</v>
       </c>
       <c r="N7" s="20">
         <v>44</v>
@@ -965,7 +966,7 @@
         <v>46</v>
       </c>
       <c r="M8">
-        <v>34.905428976361989</v>
+        <v>34.467716296422438</v>
       </c>
       <c r="N8" s="20">
         <v>44</v>
@@ -1013,7 +1014,7 @@
         <v>46</v>
       </c>
       <c r="M9">
-        <v>33.078834354332727</v>
+        <v>32.418480153017569</v>
       </c>
       <c r="N9" s="20">
         <v>44</v>
@@ -1061,7 +1062,7 @@
         <v>198</v>
       </c>
       <c r="M10">
-        <v>173.98223948728511</v>
+        <v>179.74905279769121</v>
       </c>
       <c r="N10" s="20">
         <v>296</v>
@@ -1109,7 +1110,7 @@
         <v>110</v>
       </c>
       <c r="M11">
-        <v>91.539508452843435</v>
+        <v>94.509138300523929</v>
       </c>
       <c r="N11" s="20">
         <v>44</v>
@@ -1156,8 +1157,8 @@
       <c r="L12" s="3">
         <v>68</v>
       </c>
-      <c r="M12" s="3">
-        <v>59.626571692041168</v>
+      <c r="M12">
+        <v>58.623068603283421</v>
       </c>
       <c r="N12" s="21">
         <v>44</v>
@@ -1171,7 +1172,7 @@
       </c>
       <c r="Q12" s="8">
         <f>O12-M12</f>
-        <v>-11.626571692041168</v>
+        <v>-10.623068603283421</v>
       </c>
       <c r="R12" s="8">
         <f t="shared" ref="R12:R17" si="1">N12-O12</f>
@@ -1216,7 +1217,7 @@
         <v>75</v>
       </c>
       <c r="M13">
-        <v>67.174074696381723</v>
+        <v>67.74274199969517</v>
       </c>
       <c r="N13" s="20">
         <v>44</v>
@@ -1263,8 +1264,8 @@
       <c r="L14" s="3">
         <v>70</v>
       </c>
-      <c r="M14" s="3">
-        <v>64.088337109654304</v>
+      <c r="M14">
+        <v>64.391840727219488</v>
       </c>
       <c r="N14" s="21">
         <v>44</v>
@@ -1278,7 +1279,7 @@
       </c>
       <c r="Q14" s="8">
         <f>O14-M14</f>
-        <v>-10.088337109654304</v>
+        <v>-10.391840727219488</v>
       </c>
       <c r="R14" s="8">
         <f t="shared" si="1"/>
@@ -1322,8 +1323,8 @@
       <c r="L15" s="3">
         <v>114</v>
       </c>
-      <c r="M15" s="3">
-        <v>109.9056922983319</v>
+      <c r="M15">
+        <v>110.8674542020869</v>
       </c>
       <c r="N15" s="21">
         <v>212</v>
@@ -1337,7 +1338,7 @@
       </c>
       <c r="Q15" s="8">
         <f>O15-M15</f>
-        <v>-33.9056922983319</v>
+        <v>-34.867454202086904</v>
       </c>
       <c r="R15" s="8">
         <f t="shared" si="1"/>
@@ -1381,8 +1382,8 @@
       <c r="L16" s="3">
         <v>460</v>
       </c>
-      <c r="M16" s="3">
-        <v>473.38039538904297</v>
+      <c r="M16">
+        <v>499.33953049095072</v>
       </c>
       <c r="N16" s="21">
         <v>340</v>
@@ -1396,7 +1397,7 @@
       </c>
       <c r="Q16" s="8">
         <f>O16-M16</f>
-        <v>-59.380395389042974</v>
+        <v>-85.339530490950722</v>
       </c>
       <c r="R16" s="8">
         <f t="shared" si="1"/>
@@ -1440,8 +1441,8 @@
       <c r="L17" s="3">
         <v>420</v>
       </c>
-      <c r="M17" s="3">
-        <v>420.38506339881877</v>
+      <c r="M17">
+        <v>442.80369324368343</v>
       </c>
       <c r="N17" s="21">
         <v>296</v>
@@ -1455,7 +1456,7 @@
       </c>
       <c r="Q17" s="8">
         <f>O17-M17</f>
-        <v>-22.385063398818772</v>
+        <v>-44.803693243683426</v>
       </c>
       <c r="R17" s="8">
         <f t="shared" si="1"/>
@@ -1500,7 +1501,7 @@
         <v>48</v>
       </c>
       <c r="M18">
-        <v>41.900994858328531</v>
+        <v>42.046688141426777</v>
       </c>
       <c r="N18" s="20">
         <v>44</v>
@@ -1548,9 +1549,9 @@
         <v>48</v>
       </c>
       <c r="M19">
-        <v>39.768322133434268</v>
-      </c>
-      <c r="N19" s="20">
+        <v>38.934461128219553</v>
+      </c>
+      <c r="N19" s="6">
         <v>44</v>
       </c>
       <c r="O19" s="16"/>
@@ -1568,7 +1569,7 @@
       </c>
       <c r="Q20">
         <f>SUMSQ(Q4:Q17)</f>
-        <v>5789.4474742938201</v>
+        <v>11209.143535323232</v>
       </c>
       <c r="R20">
         <f>SUMSQ(R4:R17)</f>
@@ -1592,7 +1593,15 @@
         <v>8</v>
       </c>
     </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>55.680476331125107</v>
+      </c>
+    </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M23" s="3">
+        <v>41.756478138640432</v>
+      </c>
       <c r="P23" s="12" t="s">
         <v>18</v>
       </c>
@@ -1604,17 +1613,108 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M24" s="3">
+        <v>84.929670372295817</v>
+      </c>
       <c r="P24" s="13">
         <f>SQRT(P20/P21)</f>
         <v>27.313000567495326</v>
       </c>
       <c r="Q24" s="5">
         <f>SQRT(Q20/Q21)</f>
-        <v>26.901318448855392</v>
+        <v>37.431843955586849</v>
       </c>
       <c r="R24" s="5">
         <f>SQRT(R20/R21)</f>
         <v>66.075714146727165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M25" s="3">
+        <v>37.825875345796227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>35.751889036750981</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>34.905428976361989</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>33.078834354332727</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>173.98223948728511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <v>91.539508452843435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M31" s="3">
+        <v>59.626571692041168</v>
+      </c>
+      <c r="P31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>67.174074696381723</v>
+      </c>
+      <c r="P32">
+        <v>27.313000567495326</v>
+      </c>
+      <c r="Q32">
+        <v>26.901318448855392</v>
+      </c>
+      <c r="R32">
+        <v>66.075714146727165</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M33" s="3">
+        <v>64.088337109654304</v>
+      </c>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M34" s="3">
+        <v>109.9056922983319</v>
+      </c>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M35" s="3">
+        <v>473.38039538904297</v>
+      </c>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M36" s="3">
+        <v>420.38506339881877</v>
+      </c>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>41.900994858328531</v>
+      </c>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>39.768322133434268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excluindo registro com defeito nos dados e treinando os modelos com alteração da semente
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE_Joas.xlsx
+++ b/testes/resultado_inferência_NGE_Joas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14CC622-AC90-1540-B69A-AD7938835F6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8854E7-3088-2C4E-89AF-07479BB314DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38220" yWindow="460" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -695,8 +695,8 @@
       <c r="M3">
         <v>54.605536396961817</v>
       </c>
-      <c r="N3" s="20">
-        <v>44</v>
+      <c r="N3">
+        <v>48</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="11"/>
@@ -743,8 +743,8 @@
       <c r="M4">
         <v>41.856676411395242</v>
       </c>
-      <c r="N4" s="21">
-        <v>44</v>
+      <c r="N4">
+        <v>40</v>
       </c>
       <c r="O4" s="17">
         <v>38</v>
@@ -759,7 +759,7 @@
       </c>
       <c r="R4" s="8">
         <f>N4-O4</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -802,8 +802,8 @@
       <c r="M5">
         <v>87.577477027577629</v>
       </c>
-      <c r="N5" s="21">
-        <v>46</v>
+      <c r="N5">
+        <v>86</v>
       </c>
       <c r="O5" s="17">
         <v>66</v>
@@ -817,8 +817,8 @@
         <v>-21.577477027577629</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" ref="R5:R6" si="0">N5-O5</f>
-        <v>-20</v>
+        <f>N5-O5</f>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -861,8 +861,8 @@
       <c r="M6">
         <v>37.377088243648622</v>
       </c>
-      <c r="N6" s="21">
-        <v>36</v>
+      <c r="N6">
+        <v>38</v>
       </c>
       <c r="O6" s="17">
         <v>36</v>
@@ -876,8 +876,8 @@
         <v>-1.3770882436486218</v>
       </c>
       <c r="R6" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>N6-O6</f>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -920,8 +920,8 @@
       <c r="M7">
         <v>35.401481552743753</v>
       </c>
-      <c r="N7" s="20">
-        <v>44</v>
+      <c r="N7">
+        <v>30</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="11"/>
@@ -968,8 +968,8 @@
       <c r="M8">
         <v>34.467716296422438</v>
       </c>
-      <c r="N8" s="20">
-        <v>44</v>
+      <c r="N8">
+        <v>30</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="11"/>
@@ -1016,8 +1016,8 @@
       <c r="M9">
         <v>32.418480153017569</v>
       </c>
-      <c r="N9" s="20">
-        <v>44</v>
+      <c r="N9">
+        <v>24</v>
       </c>
       <c r="O9" s="15"/>
       <c r="P9" s="11"/>
@@ -1064,8 +1064,8 @@
       <c r="M10">
         <v>179.74905279769121</v>
       </c>
-      <c r="N10" s="20">
-        <v>296</v>
+      <c r="N10">
+        <v>176</v>
       </c>
       <c r="O10" s="15"/>
       <c r="P10" s="11"/>
@@ -1112,8 +1112,8 @@
       <c r="M11">
         <v>94.509138300523929</v>
       </c>
-      <c r="N11" s="20">
-        <v>44</v>
+      <c r="N11">
+        <v>86</v>
       </c>
       <c r="O11" s="15"/>
       <c r="P11" s="11"/>
@@ -1160,8 +1160,8 @@
       <c r="M12">
         <v>58.623068603283421</v>
       </c>
-      <c r="N12" s="21">
-        <v>44</v>
+      <c r="N12">
+        <v>72</v>
       </c>
       <c r="O12" s="17">
         <v>48</v>
@@ -1175,8 +1175,8 @@
         <v>-10.623068603283421</v>
       </c>
       <c r="R12" s="8">
-        <f t="shared" ref="R12:R17" si="1">N12-O12</f>
-        <v>-4</v>
+        <f>N12-O12</f>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1219,8 +1219,8 @@
       <c r="M13">
         <v>67.74274199969517</v>
       </c>
-      <c r="N13" s="20">
-        <v>44</v>
+      <c r="N13">
+        <v>68</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="11"/>
@@ -1267,8 +1267,8 @@
       <c r="M14">
         <v>64.391840727219488</v>
       </c>
-      <c r="N14" s="21">
-        <v>44</v>
+      <c r="N14">
+        <v>68</v>
       </c>
       <c r="O14" s="17">
         <v>54</v>
@@ -1282,8 +1282,8 @@
         <v>-10.391840727219488</v>
       </c>
       <c r="R14" s="8">
-        <f t="shared" si="1"/>
-        <v>-10</v>
+        <f>N14-O14</f>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1326,8 +1326,8 @@
       <c r="M15">
         <v>110.8674542020869</v>
       </c>
-      <c r="N15" s="21">
-        <v>212</v>
+      <c r="N15">
+        <v>110</v>
       </c>
       <c r="O15" s="17">
         <v>76</v>
@@ -1341,8 +1341,8 @@
         <v>-34.867454202086904</v>
       </c>
       <c r="R15" s="8">
-        <f t="shared" si="1"/>
-        <v>136</v>
+        <f>N15-O15</f>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1385,7 +1385,7 @@
       <c r="M16">
         <v>499.33953049095072</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16">
         <v>340</v>
       </c>
       <c r="O16" s="17">
@@ -1400,7 +1400,7 @@
         <v>-85.339530490950722</v>
       </c>
       <c r="R16" s="8">
-        <f t="shared" si="1"/>
+        <f>N16-O16</f>
         <v>-74</v>
       </c>
     </row>
@@ -1444,8 +1444,8 @@
       <c r="M17">
         <v>442.80369324368343</v>
       </c>
-      <c r="N17" s="21">
-        <v>296</v>
+      <c r="N17">
+        <v>340</v>
       </c>
       <c r="O17" s="17">
         <v>398</v>
@@ -1459,8 +1459,8 @@
         <v>-44.803693243683426</v>
       </c>
       <c r="R17" s="8">
-        <f t="shared" si="1"/>
-        <v>-102</v>
+        <f>N17-O17</f>
+        <v>-58</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1503,8 +1503,8 @@
       <c r="M18">
         <v>42.046688141426777</v>
       </c>
-      <c r="N18" s="20">
-        <v>44</v>
+      <c r="N18">
+        <v>40</v>
       </c>
       <c r="O18" s="15"/>
       <c r="P18" s="9"/>
@@ -1551,8 +1551,8 @@
       <c r="M19">
         <v>38.934461128219553</v>
       </c>
-      <c r="N19" s="6">
-        <v>44</v>
+      <c r="N19">
+        <v>30</v>
       </c>
       <c r="O19" s="16"/>
       <c r="P19" s="9"/>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="R20">
         <f>SUMSQ(R4:R17)</f>
-        <v>34928</v>
+        <v>11176</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -1597,11 +1597,17 @@
       <c r="M22">
         <v>55.680476331125107</v>
       </c>
+      <c r="N22" s="20">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M23" s="3">
         <v>41.756478138640432</v>
       </c>
+      <c r="N23" s="21">
+        <v>44</v>
+      </c>
       <c r="P23" s="12" t="s">
         <v>18</v>
       </c>
@@ -1616,6 +1622,9 @@
       <c r="M24" s="3">
         <v>84.929670372295817</v>
       </c>
+      <c r="N24" s="21">
+        <v>46</v>
+      </c>
       <c r="P24" s="13">
         <f>SQRT(P20/P21)</f>
         <v>27.313000567495326</v>
@@ -1626,43 +1635,64 @@
       </c>
       <c r="R24" s="5">
         <f>SQRT(R20/R21)</f>
-        <v>66.075714146727165</v>
+        <v>37.376463182061514</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M25" s="3">
         <v>37.825875345796227</v>
       </c>
+      <c r="N25" s="21">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M26">
         <v>35.751889036750981</v>
       </c>
+      <c r="N26" s="20">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M27">
         <v>34.905428976361989</v>
       </c>
+      <c r="N27" s="20">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M28">
         <v>33.078834354332727</v>
       </c>
+      <c r="N28" s="20">
+        <v>44</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M29">
         <v>173.98223948728511</v>
       </c>
+      <c r="N29" s="20">
+        <v>296</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M30">
         <v>91.539508452843435</v>
       </c>
+      <c r="N30" s="20">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M31" s="3">
         <v>59.626571692041168</v>
       </c>
+      <c r="N31" s="21">
+        <v>44</v>
+      </c>
       <c r="P31" t="s">
         <v>18</v>
       </c>
@@ -1677,6 +1707,9 @@
       <c r="M32">
         <v>67.174074696381723</v>
       </c>
+      <c r="N32" s="20">
+        <v>44</v>
+      </c>
       <c r="P32">
         <v>27.313000567495326</v>
       </c>
@@ -1687,34 +1720,52 @@
         <v>66.075714146727165</v>
       </c>
     </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M33" s="3">
         <v>64.088337109654304</v>
       </c>
-    </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="N33" s="21">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M34" s="3">
         <v>109.9056922983319</v>
       </c>
-    </row>
-    <row r="35" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="N34" s="21">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M35" s="3">
         <v>473.38039538904297</v>
       </c>
-    </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="N35" s="21">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="36" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M36" s="3">
         <v>420.38506339881877</v>
       </c>
-    </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="N36" s="21">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M37">
         <v>41.900994858328531</v>
       </c>
-    </row>
-    <row r="38" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M38">
         <v>39.768322133434268</v>
+      </c>
+      <c r="N38" s="6">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incluindo coluna tipo demanda para poder fazer split dataframe para treinamento com estratificação dessa nova coluna
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE_Joas.xlsx
+++ b/testes/resultado_inferência_NGE_Joas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8854E7-3088-2C4E-89AF-07479BB314DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C62775-FF76-B14B-96DB-7D10699F91E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38220" yWindow="460" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -693,7 +693,7 @@
         <v>48</v>
       </c>
       <c r="M3">
-        <v>54.605536396961817</v>
+        <v>54.46713274517316</v>
       </c>
       <c r="N3">
         <v>48</v>
@@ -741,7 +741,7 @@
         <v>48</v>
       </c>
       <c r="M4">
-        <v>41.856676411395242</v>
+        <v>39.790391641953093</v>
       </c>
       <c r="N4">
         <v>40</v>
@@ -755,7 +755,7 @@
       </c>
       <c r="Q4" s="8">
         <f>O4-M4</f>
-        <v>-3.8566764113952416</v>
+        <v>-1.790391641953093</v>
       </c>
       <c r="R4" s="8">
         <f>N4-O4</f>
@@ -800,7 +800,7 @@
         <v>98</v>
       </c>
       <c r="M5">
-        <v>87.577477027577629</v>
+        <v>77.295274042005587</v>
       </c>
       <c r="N5">
         <v>86</v>
@@ -814,7 +814,7 @@
       </c>
       <c r="Q5" s="8">
         <f>O5-M5</f>
-        <v>-21.577477027577629</v>
+        <v>-11.295274042005587</v>
       </c>
       <c r="R5" s="8">
         <f>N5-O5</f>
@@ -859,7 +859,7 @@
         <v>48</v>
       </c>
       <c r="M6">
-        <v>37.377088243648622</v>
+        <v>37.374947253641352</v>
       </c>
       <c r="N6">
         <v>38</v>
@@ -873,7 +873,7 @@
       </c>
       <c r="Q6" s="8">
         <f>O6-M6</f>
-        <v>-1.3770882436486218</v>
+        <v>-1.3749472536413521</v>
       </c>
       <c r="R6" s="8">
         <f>N6-O6</f>
@@ -918,7 +918,7 @@
         <v>46</v>
       </c>
       <c r="M7">
-        <v>35.401481552743753</v>
+        <v>31.296339673006749</v>
       </c>
       <c r="N7">
         <v>30</v>
@@ -966,7 +966,7 @@
         <v>46</v>
       </c>
       <c r="M8">
-        <v>34.467716296422438</v>
+        <v>30.431195639155501</v>
       </c>
       <c r="N8">
         <v>30</v>
@@ -1014,7 +1014,7 @@
         <v>46</v>
       </c>
       <c r="M9">
-        <v>32.418480153017569</v>
+        <v>28.93465931102369</v>
       </c>
       <c r="N9">
         <v>24</v>
@@ -1062,7 +1062,7 @@
         <v>198</v>
       </c>
       <c r="M10">
-        <v>179.74905279769121</v>
+        <v>171.9960647176099</v>
       </c>
       <c r="N10">
         <v>176</v>
@@ -1110,7 +1110,7 @@
         <v>110</v>
       </c>
       <c r="M11">
-        <v>94.509138300523929</v>
+        <v>87.903185770664876</v>
       </c>
       <c r="N11">
         <v>86</v>
@@ -1158,7 +1158,7 @@
         <v>68</v>
       </c>
       <c r="M12">
-        <v>58.623068603283421</v>
+        <v>59.890885753675519</v>
       </c>
       <c r="N12">
         <v>72</v>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="Q12" s="8">
         <f>O12-M12</f>
-        <v>-10.623068603283421</v>
+        <v>-11.890885753675519</v>
       </c>
       <c r="R12" s="8">
         <f>N12-O12</f>
@@ -1217,7 +1217,7 @@
         <v>75</v>
       </c>
       <c r="M13">
-        <v>67.74274199969517</v>
+        <v>63.486656447616639</v>
       </c>
       <c r="N13">
         <v>68</v>
@@ -1265,7 +1265,7 @@
         <v>70</v>
       </c>
       <c r="M14">
-        <v>64.391840727219488</v>
+        <v>61.617732914796079</v>
       </c>
       <c r="N14">
         <v>68</v>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="Q14" s="8">
         <f>O14-M14</f>
-        <v>-10.391840727219488</v>
+        <v>-7.6177329147960791</v>
       </c>
       <c r="R14" s="8">
         <f>N14-O14</f>
@@ -1324,7 +1324,7 @@
         <v>114</v>
       </c>
       <c r="M15">
-        <v>110.8674542020869</v>
+        <v>136.22046273298781</v>
       </c>
       <c r="N15">
         <v>110</v>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="Q15" s="8">
         <f>O15-M15</f>
-        <v>-34.867454202086904</v>
+        <v>-60.220462732987812</v>
       </c>
       <c r="R15" s="8">
         <f>N15-O15</f>
@@ -1383,7 +1383,7 @@
         <v>460</v>
       </c>
       <c r="M16">
-        <v>499.33953049095072</v>
+        <v>462.14463659982363</v>
       </c>
       <c r="N16">
         <v>340</v>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="Q16" s="8">
         <f>O16-M16</f>
-        <v>-85.339530490950722</v>
+        <v>-48.144636599823627</v>
       </c>
       <c r="R16" s="8">
         <f>N16-O16</f>
@@ -1442,7 +1442,7 @@
         <v>420</v>
       </c>
       <c r="M17">
-        <v>442.80369324368343</v>
+        <v>407.9055187250251</v>
       </c>
       <c r="N17">
         <v>340</v>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="Q17" s="8">
         <f>O17-M17</f>
-        <v>-44.803693243683426</v>
+        <v>-9.9055187250251038</v>
       </c>
       <c r="R17" s="8">
         <f>N17-O17</f>
@@ -1501,7 +1501,7 @@
         <v>48</v>
       </c>
       <c r="M18">
-        <v>42.046688141426777</v>
+        <v>37.290223656749582</v>
       </c>
       <c r="N18">
         <v>40</v>
@@ -1549,7 +1549,7 @@
         <v>48</v>
       </c>
       <c r="M19">
-        <v>38.934461128219553</v>
+        <v>37.380204494397667</v>
       </c>
       <c r="N19">
         <v>30</v>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="Q20">
         <f>SUMSQ(Q4:Q17)</f>
-        <v>11209.143535323232</v>
+        <v>6374.6316829500811</v>
       </c>
       <c r="R20">
         <f>SUMSQ(R4:R17)</f>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="Q24" s="5">
         <f>SQRT(Q20/Q21)</f>
-        <v>37.431843955586849</v>
+        <v>28.228158997156726</v>
       </c>
       <c r="R24" s="5">
         <f>SQRT(R20/R21)</f>

</xml_diff>

<commit_message>
refazendo criterio para tipo de demanda e mudando semente randomica
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE_Joas.xlsx
+++ b/testes/resultado_inferência_NGE_Joas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C62775-FF76-B14B-96DB-7D10699F91E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610BA5C6-3B79-6241-9A39-7CF7DEDA2E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38220" yWindow="460" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Modelo 2 - Reg Linear</t>
+  </si>
+  <si>
+    <t>Modelo 3 - Forest</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,7 +598,7 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q1" s="19" t="s">
         <v>20</v>
@@ -744,7 +747,7 @@
         <v>39.790391641953093</v>
       </c>
       <c r="N4">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="O4" s="17">
         <v>38</v>
@@ -759,7 +762,7 @@
       </c>
       <c r="R4" s="8">
         <f>N4-O4</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -862,7 +865,7 @@
         <v>37.374947253641352</v>
       </c>
       <c r="N6">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O6" s="17">
         <v>36</v>
@@ -877,7 +880,7 @@
       </c>
       <c r="R6" s="8">
         <f>N6-O6</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -1017,7 +1020,7 @@
         <v>28.93465931102369</v>
       </c>
       <c r="N9">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="O9" s="15"/>
       <c r="P9" s="11"/>
@@ -1113,7 +1116,7 @@
         <v>87.903185770664876</v>
       </c>
       <c r="N11">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O11" s="15"/>
       <c r="P11" s="11"/>
@@ -1220,7 +1223,7 @@
         <v>63.486656447616639</v>
       </c>
       <c r="N13">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="11"/>
@@ -1327,7 +1330,7 @@
         <v>136.22046273298781</v>
       </c>
       <c r="N15">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="O15" s="17">
         <v>76</v>
@@ -1342,7 +1345,7 @@
       </c>
       <c r="R15" s="8">
         <f>N15-O15</f>
-        <v>34</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1391,18 +1394,9 @@
       <c r="O16" s="17">
         <v>414</v>
       </c>
-      <c r="P16" s="11">
-        <f>O16-L16</f>
-        <v>-46</v>
-      </c>
-      <c r="Q16" s="8">
-        <f>O16-M16</f>
-        <v>-48.144636599823627</v>
-      </c>
-      <c r="R16" s="8">
-        <f>N16-O16</f>
-        <v>-74</v>
-      </c>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -1445,23 +1439,14 @@
         <v>407.9055187250251</v>
       </c>
       <c r="N17">
-        <v>340</v>
+        <v>212</v>
       </c>
       <c r="O17" s="17">
         <v>398</v>
       </c>
-      <c r="P17" s="11">
-        <f>O17-L17</f>
-        <v>-22</v>
-      </c>
-      <c r="Q17" s="8">
-        <f>O17-M17</f>
-        <v>-9.9055187250251038</v>
-      </c>
-      <c r="R17" s="8">
-        <f>N17-O17</f>
-        <v>-58</v>
-      </c>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1504,7 +1489,7 @@
         <v>37.290223656749582</v>
       </c>
       <c r="N18">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="O18" s="15"/>
       <c r="P18" s="9"/>
@@ -1552,7 +1537,7 @@
         <v>37.380204494397667</v>
       </c>
       <c r="N19">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="O19" s="16"/>
       <c r="P19" s="9"/>
@@ -1565,15 +1550,15 @@
       </c>
       <c r="P20">
         <f>SUMSQ(P3:P19)</f>
-        <v>5968</v>
+        <v>3368</v>
       </c>
       <c r="Q20">
         <f>SUMSQ(Q4:Q17)</f>
-        <v>6374.6316829500811</v>
+        <v>3958.6063484091815</v>
       </c>
       <c r="R20">
         <f>SUMSQ(R4:R17)</f>
-        <v>11176</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -1586,11 +1571,11 @@
       </c>
       <c r="Q21">
         <f>COUNT(P3:P19)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R21">
         <f>COUNT(Q3:Q19)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -1627,15 +1612,15 @@
       </c>
       <c r="P24" s="13">
         <f>SQRT(P20/P21)</f>
-        <v>27.313000567495326</v>
+        <v>20.518284528683193</v>
       </c>
       <c r="Q24" s="5">
         <f>SQRT(Q20/Q21)</f>
-        <v>28.228158997156726</v>
+        <v>25.685944108302962</v>
       </c>
       <c r="R24" s="5">
         <f>SQRT(R20/R21)</f>
-        <v>37.376463182061514</v>
+        <v>18.421002506197464</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ajustes para melhorar acuracia
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE_Joas.xlsx
+++ b/testes/resultado_inferência_NGE_Joas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610BA5C6-3B79-6241-9A39-7CF7DEDA2E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4044B0B-A030-974C-8878-6924712C0D8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38220" yWindow="460" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -124,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +179,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -232,11 +238,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -275,6 +290,25 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,37 +611,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="19" customWidth="1"/>
-    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="17" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="19" max="19" width="19" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M1" s="19" t="s">
         <v>20</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="28">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,20 +688,31 @@
         <v>11</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="R2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W2" s="28">
+        <v>74</v>
+      </c>
+      <c r="X2" s="28">
+        <v>235806</v>
+      </c>
+      <c r="AC2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -701,12 +755,27 @@
       <c r="N3">
         <v>48</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="W3">
+        <v>48</v>
+      </c>
+      <c r="X3">
+        <v>235832</v>
+      </c>
+      <c r="AB3" s="28">
+        <v>68</v>
+      </c>
+      <c r="AC3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -749,23 +818,35 @@
       <c r="N4">
         <v>46</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="17">
         <v>38</v>
       </c>
-      <c r="P4" s="11">
-        <f>O4-L4</f>
+      <c r="R4" s="11">
+        <f>Q4-L4</f>
         <v>-10</v>
       </c>
-      <c r="Q4" s="8">
-        <f>O4-M4</f>
+      <c r="S4" s="8">
+        <f>Q4-M4</f>
         <v>-1.790391641953093</v>
       </c>
-      <c r="R4" s="8">
-        <f>N4-O4</f>
+      <c r="T4" s="8">
+        <f>N4-Q4</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W4" s="28">
+        <v>68</v>
+      </c>
+      <c r="X4" s="28">
+        <v>235874</v>
+      </c>
+      <c r="AC4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -808,23 +889,35 @@
       <c r="N5">
         <v>86</v>
       </c>
-      <c r="O5" s="17">
+      <c r="O5">
+        <v>86</v>
+      </c>
+      <c r="Q5" s="17">
         <v>66</v>
       </c>
-      <c r="P5" s="11">
-        <f>O5-L5</f>
+      <c r="R5" s="11">
+        <f>Q5-L5</f>
         <v>-32</v>
       </c>
-      <c r="Q5" s="8">
-        <f>O5-M5</f>
+      <c r="S5" s="8">
+        <f>Q5-M5</f>
         <v>-11.295274042005587</v>
       </c>
-      <c r="R5" s="8">
-        <f>N5-O5</f>
+      <c r="T5" s="8">
+        <f>N5-Q5</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W5">
+        <v>46</v>
+      </c>
+      <c r="X5">
+        <v>235876</v>
+      </c>
+      <c r="AC5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -867,23 +960,35 @@
       <c r="N6">
         <v>40</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="17">
         <v>36</v>
       </c>
-      <c r="P6" s="11">
-        <f>O6-L6</f>
+      <c r="R6" s="11">
+        <f>Q6-L6</f>
         <v>-12</v>
       </c>
-      <c r="Q6" s="8">
-        <f>O6-M6</f>
+      <c r="S6" s="8">
+        <f>Q6-M6</f>
         <v>-1.3749472536413521</v>
       </c>
-      <c r="R6" s="8">
-        <f>N6-O6</f>
+      <c r="T6" s="8">
+        <f>N6-Q6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W6">
+        <v>86</v>
+      </c>
+      <c r="X6">
+        <v>235878</v>
+      </c>
+      <c r="AC6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -926,12 +1031,24 @@
       <c r="N7">
         <v>30</v>
       </c>
-      <c r="O7" s="15"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="W7">
+        <v>40</v>
+      </c>
+      <c r="X7">
+        <v>235880</v>
+      </c>
+      <c r="AC7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -974,12 +1091,24 @@
       <c r="N8">
         <v>30</v>
       </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="W8">
+        <v>30</v>
+      </c>
+      <c r="X8">
+        <v>235881</v>
+      </c>
+      <c r="AC8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1020,14 +1149,26 @@
         <v>28.93465931102369</v>
       </c>
       <c r="N9">
+        <v>28</v>
+      </c>
+      <c r="O9">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="W9">
         <v>30</v>
       </c>
-      <c r="O9" s="15"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="X9">
+        <v>235883</v>
+      </c>
+      <c r="AC9">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1070,12 +1211,24 @@
       <c r="N10">
         <v>176</v>
       </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>176</v>
+      </c>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="W10">
+        <v>28</v>
+      </c>
+      <c r="X10">
+        <v>235882</v>
+      </c>
+      <c r="AC10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1116,14 +1269,26 @@
         <v>87.903185770664876</v>
       </c>
       <c r="N11">
+        <v>86</v>
+      </c>
+      <c r="O11">
         <v>84</v>
       </c>
-      <c r="O11" s="15"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q11" s="15"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="W11">
+        <v>176</v>
+      </c>
+      <c r="X11">
+        <v>235798</v>
+      </c>
+      <c r="AC11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1166,23 +1331,35 @@
       <c r="N12">
         <v>72</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12">
+        <v>72</v>
+      </c>
+      <c r="Q12" s="17">
         <v>48</v>
       </c>
-      <c r="P12" s="11">
-        <f>O12-L12</f>
+      <c r="R12" s="11">
+        <f>Q12-L12</f>
         <v>-20</v>
       </c>
-      <c r="Q12" s="8">
-        <f>O12-M12</f>
+      <c r="S12" s="8">
+        <f>Q12-M12</f>
         <v>-11.890885753675519</v>
       </c>
-      <c r="R12" s="8">
-        <f>N12-O12</f>
+      <c r="T12" s="8">
+        <f>N12-Q12</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W12">
+        <v>84</v>
+      </c>
+      <c r="X12">
+        <v>235905</v>
+      </c>
+      <c r="AC12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1225,12 +1402,24 @@
       <c r="N13">
         <v>48</v>
       </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>48</v>
+      </c>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="W13">
+        <v>72</v>
+      </c>
+      <c r="X13">
+        <v>235909</v>
+      </c>
+      <c r="AC13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1273,23 +1462,35 @@
       <c r="N14">
         <v>68</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14">
+        <v>68</v>
+      </c>
+      <c r="Q14" s="17">
         <v>54</v>
       </c>
-      <c r="P14" s="11">
-        <f>O14-L14</f>
+      <c r="R14" s="11">
+        <f>Q14-L14</f>
         <v>-16</v>
       </c>
-      <c r="Q14" s="8">
-        <f>O14-M14</f>
+      <c r="S14" s="8">
+        <f>Q14-M14</f>
         <v>-7.6177329147960791</v>
       </c>
-      <c r="R14" s="8">
-        <f>N14-O14</f>
+      <c r="T14" s="8">
+        <f>N14-Q14</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W14">
+        <v>48</v>
+      </c>
+      <c r="X14">
+        <v>235964</v>
+      </c>
+      <c r="AC14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1330,25 +1531,37 @@
         <v>136.22046273298781</v>
       </c>
       <c r="N15">
-        <v>48</v>
-      </c>
-      <c r="O15" s="17">
+        <v>40</v>
+      </c>
+      <c r="O15">
+        <v>40</v>
+      </c>
+      <c r="Q15" s="17">
         <v>76</v>
       </c>
-      <c r="P15" s="11">
-        <f>O15-L15</f>
+      <c r="R15" s="11">
+        <f>Q15-L15</f>
         <v>-38</v>
       </c>
-      <c r="Q15" s="8">
-        <f>O15-M15</f>
+      <c r="S15" s="8">
+        <f>Q15-M15</f>
         <v>-60.220462732987812</v>
       </c>
-      <c r="R15" s="8">
-        <f>N15-O15</f>
-        <v>-28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T15" s="8">
+        <f>N15-Q15</f>
+        <v>-36</v>
+      </c>
+      <c r="W15">
+        <v>68</v>
+      </c>
+      <c r="X15">
+        <v>235979</v>
+      </c>
+      <c r="AC15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1391,14 +1604,38 @@
       <c r="N16">
         <v>340</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16">
+        <v>340</v>
+      </c>
+      <c r="Q16" s="17">
         <v>414</v>
       </c>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R16" s="11">
+        <f t="shared" ref="R16:R17" si="0">Q16-L16</f>
+        <v>-46</v>
+      </c>
+      <c r="S16" s="8">
+        <f t="shared" ref="S16:S17" si="1">Q16-M16</f>
+        <v>-48.144636599823627</v>
+      </c>
+      <c r="T16" s="8">
+        <f t="shared" ref="T16:T17" si="2">N16-Q16</f>
+        <v>-74</v>
+      </c>
+      <c r="W16">
+        <v>40</v>
+      </c>
+      <c r="X16">
+        <v>235980</v>
+      </c>
+      <c r="AB16" s="28">
+        <v>46</v>
+      </c>
+      <c r="AC16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1439,16 +1676,40 @@
         <v>407.9055187250251</v>
       </c>
       <c r="N17">
-        <v>212</v>
-      </c>
-      <c r="O17" s="17">
+        <v>340</v>
+      </c>
+      <c r="O17">
+        <v>340</v>
+      </c>
+      <c r="Q17" s="17">
         <v>398</v>
       </c>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R17" s="11">
+        <f t="shared" si="0"/>
+        <v>-22</v>
+      </c>
+      <c r="S17" s="8">
+        <f t="shared" si="1"/>
+        <v>-9.9055187250251038</v>
+      </c>
+      <c r="T17" s="8">
+        <f t="shared" si="2"/>
+        <v>-58</v>
+      </c>
+      <c r="W17" s="28">
+        <v>46</v>
+      </c>
+      <c r="X17" s="28">
+        <v>235981</v>
+      </c>
+      <c r="AB17" s="28">
+        <v>44</v>
+      </c>
+      <c r="AC17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1491,12 +1752,24 @@
       <c r="N18">
         <v>46</v>
       </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="O18">
+        <v>46</v>
+      </c>
+      <c r="Q18" s="15"/>
       <c r="R18" s="9"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="W18" s="28">
+        <v>44</v>
+      </c>
+      <c r="X18" s="28">
+        <v>235984</v>
+      </c>
+      <c r="AC18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1539,91 +1812,129 @@
       <c r="N19">
         <v>40</v>
       </c>
-      <c r="O19" s="16"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="O19">
+        <v>40</v>
+      </c>
+      <c r="Q19" s="16"/>
       <c r="R19" s="9"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="O20" t="s">
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="W19">
+        <v>340</v>
+      </c>
+      <c r="X19">
+        <v>235985</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Q20" t="s">
         <v>14</v>
       </c>
-      <c r="P20">
-        <f>SUMSQ(P3:P19)</f>
-        <v>3368</v>
-      </c>
-      <c r="Q20">
-        <f>SUMSQ(Q4:Q17)</f>
-        <v>3958.6063484091815</v>
-      </c>
       <c r="R20">
-        <f>SUMSQ(R4:R17)</f>
-        <v>2036</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="O21" t="s">
+        <f>SUMSQ(R3:R19)</f>
+        <v>5968</v>
+      </c>
+      <c r="S20">
+        <f>SUMSQ(S4:S17)</f>
+        <v>6374.6316829500811</v>
+      </c>
+      <c r="T20">
+        <f>SUMSQ(T4:T17)</f>
+        <v>11388</v>
+      </c>
+      <c r="W20">
+        <v>340</v>
+      </c>
+      <c r="X20">
+        <v>235986</v>
+      </c>
+      <c r="AB20" s="28">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Q21" t="s">
         <v>15</v>
-      </c>
-      <c r="P21">
-        <f>COUNT(O3:O19)</f>
-        <v>8</v>
-      </c>
-      <c r="Q21">
-        <f>COUNT(P3:P19)</f>
-        <v>6</v>
       </c>
       <c r="R21">
         <f>COUNT(Q3:Q19)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="S21">
+        <f>COUNT(R3:R19)</f>
+        <v>8</v>
+      </c>
+      <c r="T21">
+        <f>COUNT(S3:S19)</f>
+        <v>8</v>
+      </c>
+      <c r="W21" s="28">
+        <v>46</v>
+      </c>
+      <c r="X21" s="28">
+        <v>235983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M22">
         <v>55.680476331125107</v>
       </c>
       <c r="N22" s="20">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="W22">
+        <v>46</v>
+      </c>
+      <c r="X22">
+        <v>236021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M23" s="3">
         <v>41.756478138640432</v>
       </c>
       <c r="N23" s="21">
         <v>44</v>
       </c>
-      <c r="P23" s="12" t="s">
+      <c r="R23" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Q23" s="4" t="s">
+      <c r="S23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W23">
+        <v>40</v>
+      </c>
+      <c r="X23">
+        <v>236025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M24" s="3">
         <v>84.929670372295817</v>
       </c>
       <c r="N24" s="21">
         <v>46</v>
       </c>
-      <c r="P24" s="13">
-        <f>SQRT(P20/P21)</f>
-        <v>20.518284528683193</v>
-      </c>
-      <c r="Q24" s="5">
-        <f>SQRT(Q20/Q21)</f>
-        <v>25.685944108302962</v>
-      </c>
-      <c r="R24" s="5">
+      <c r="R24" s="13">
         <f>SQRT(R20/R21)</f>
-        <v>18.421002506197464</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+        <v>27.313000567495326</v>
+      </c>
+      <c r="S24" s="5">
+        <f>SQRT(S20/S21)</f>
+        <v>28.228158997156726</v>
+      </c>
+      <c r="T24" s="5">
+        <f>SQRT(T20/T21)</f>
+        <v>37.729298959826963</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M25" s="3">
         <v>37.825875345796227</v>
       </c>
@@ -1631,7 +1942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M26">
         <v>35.751889036750981</v>
       </c>
@@ -1639,7 +1950,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M27">
         <v>34.905428976361989</v>
       </c>
@@ -1647,7 +1958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M28">
         <v>33.078834354332727</v>
       </c>
@@ -1655,57 +1966,75 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M29">
         <v>173.98223948728511</v>
       </c>
       <c r="N29" s="20">
         <v>296</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R29" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="S29" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="T29" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M30">
         <v>91.539508452843435</v>
       </c>
       <c r="N30" s="20">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R30" s="24">
+        <v>20.518284528683193</v>
+      </c>
+      <c r="S30" s="25">
+        <v>25.685944108302962</v>
+      </c>
+      <c r="T30" s="25">
+        <v>20.607442021431645</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M31" s="3">
         <v>59.626571692041168</v>
       </c>
       <c r="N31" s="21">
         <v>44</v>
       </c>
-      <c r="P31" t="s">
+      <c r="R31" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="S31" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="R31" t="s">
+      <c r="T31" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M32">
         <v>67.174074696381723</v>
       </c>
       <c r="N32" s="20">
         <v>44</v>
       </c>
-      <c r="P32">
+      <c r="R32" s="24">
         <v>27.313000567495326</v>
       </c>
-      <c r="Q32">
+      <c r="S32" s="25">
         <v>26.901318448855392</v>
       </c>
-      <c r="R32">
+      <c r="T32" s="25">
         <v>66.075714146727165</v>
       </c>
     </row>
-    <row r="33" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M33" s="3">
         <v>64.088337109654304</v>
       </c>
@@ -1713,7 +2042,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M34" s="3">
         <v>109.9056922983319</v>
       </c>
@@ -1721,7 +2050,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M35" s="3">
         <v>473.38039538904297</v>
       </c>
@@ -1729,7 +2058,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="36" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M36" s="3">
         <v>420.38506339881877</v>
       </c>
@@ -1737,21 +2066,25 @@
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M37">
         <v>41.900994858328531</v>
       </c>
       <c r="N37" s="20">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+    </row>
+    <row r="38" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M38">
         <v>39.768322133434268</v>
       </c>
       <c r="N38" s="6">
         <v>44</v>
       </c>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adicioando dados de entrada e mudando arquiv excel de entrada
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE_Joas.xlsx
+++ b/testes/resultado_inferência_NGE_Joas.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4044B0B-A030-974C-8878-6924712C0D8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6726EC26-37EF-FA45-B3E1-9E1139DB65A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38220" yWindow="460" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35280" yWindow="1580" windowWidth="36700" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inferencia por IA" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="95">
   <si>
     <t>id</t>
   </si>
@@ -96,13 +97,232 @@
   </si>
   <si>
     <t>Modelo 3 - Forest</t>
+  </si>
+  <si>
+    <t>235874</t>
+  </si>
+  <si>
+    <t>235881</t>
+  </si>
+  <si>
+    <t>235883</t>
+  </si>
+  <si>
+    <t>235882</t>
+  </si>
+  <si>
+    <t>235798</t>
+  </si>
+  <si>
+    <t>235964</t>
+  </si>
+  <si>
+    <t>236025</t>
+  </si>
+  <si>
+    <t>236105</t>
+  </si>
+  <si>
+    <t>236123</t>
+  </si>
+  <si>
+    <t>235382</t>
+  </si>
+  <si>
+    <t>233900</t>
+  </si>
+  <si>
+    <t>235513</t>
+  </si>
+  <si>
+    <t>235514</t>
+  </si>
+  <si>
+    <t>235700</t>
+  </si>
+  <si>
+    <t>235701</t>
+  </si>
+  <si>
+    <t>235710</t>
+  </si>
+  <si>
+    <t>235813</t>
+  </si>
+  <si>
+    <t>235512</t>
+  </si>
+  <si>
+    <t>235520</t>
+  </si>
+  <si>
+    <t>235534</t>
+  </si>
+  <si>
+    <t>235650</t>
+  </si>
+  <si>
+    <t>235652</t>
+  </si>
+  <si>
+    <t>235651</t>
+  </si>
+  <si>
+    <t>235664</t>
+  </si>
+  <si>
+    <t>235665</t>
+  </si>
+  <si>
+    <t>235142</t>
+  </si>
+  <si>
+    <t>235806</t>
+  </si>
+  <si>
+    <t>235810</t>
+  </si>
+  <si>
+    <t>235811</t>
+  </si>
+  <si>
+    <t>235812</t>
+  </si>
+  <si>
+    <t>235831</t>
+  </si>
+  <si>
+    <t>235832</t>
+  </si>
+  <si>
+    <t>235876</t>
+  </si>
+  <si>
+    <t>235878</t>
+  </si>
+  <si>
+    <t>235880</t>
+  </si>
+  <si>
+    <t>235905</t>
+  </si>
+  <si>
+    <t>235909</t>
+  </si>
+  <si>
+    <t>235979</t>
+  </si>
+  <si>
+    <t>235980</t>
+  </si>
+  <si>
+    <t>235981</t>
+  </si>
+  <si>
+    <t>235981B</t>
+  </si>
+  <si>
+    <t>235984</t>
+  </si>
+  <si>
+    <t>235984B</t>
+  </si>
+  <si>
+    <t>235985</t>
+  </si>
+  <si>
+    <t>235986</t>
+  </si>
+  <si>
+    <t>235983</t>
+  </si>
+  <si>
+    <t>235983B</t>
+  </si>
+  <si>
+    <t>236021</t>
+  </si>
+  <si>
+    <t>001/2020</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>398</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Nº DA PLANILHA</t>
+  </si>
+  <si>
+    <t>Nº de páginas finais</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +343,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,12 +403,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -185,8 +413,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -247,11 +499,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -269,7 +579,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -281,10 +590,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,11 +610,41 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC38"/>
+  <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -628,16 +964,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="15" t="s">
         <v>20</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="15" t="s">
         <v>19</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -646,7 +982,7 @@
       <c r="X1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB1" s="28">
+      <c r="AB1" s="24">
         <v>74</v>
       </c>
     </row>
@@ -687,13 +1023,13 @@
       <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="14" t="s">
+      <c r="N2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>13</v>
       </c>
       <c r="S2" s="7" t="s">
@@ -702,10 +1038,10 @@
       <c r="T2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="28">
+      <c r="W2" s="24">
         <v>74</v>
       </c>
-      <c r="X2" s="28">
+      <c r="X2" s="24">
         <v>235806</v>
       </c>
       <c r="AC2">
@@ -759,7 +1095,7 @@
         <v>48</v>
       </c>
       <c r="Q3" s="15"/>
-      <c r="R3" s="11"/>
+      <c r="R3" s="10"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="W3">
@@ -768,7 +1104,7 @@
       <c r="X3">
         <v>235832</v>
       </c>
-      <c r="AB3" s="28">
+      <c r="AB3" s="24">
         <v>68</v>
       </c>
       <c r="AC3">
@@ -806,7 +1142,7 @@
       <c r="J4" s="3">
         <v>29</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="14">
         <v>30</v>
       </c>
       <c r="L4" s="3">
@@ -821,25 +1157,25 @@
       <c r="O4">
         <v>46</v>
       </c>
-      <c r="Q4" s="17">
-        <v>38</v>
-      </c>
-      <c r="R4" s="11">
-        <f>Q4-L4</f>
-        <v>-10</v>
+      <c r="Q4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="10">
+        <f>L4-Q4</f>
+        <v>10</v>
       </c>
       <c r="S4" s="8">
-        <f>Q4-M4</f>
-        <v>-1.790391641953093</v>
+        <f>M4-Q4</f>
+        <v>1.790391641953093</v>
       </c>
       <c r="T4" s="8">
         <f>N4-Q4</f>
         <v>8</v>
       </c>
-      <c r="W4" s="28">
+      <c r="W4" s="24">
         <v>68</v>
       </c>
-      <c r="X4" s="28">
+      <c r="X4" s="24">
         <v>235874</v>
       </c>
       <c r="AC4">
@@ -877,7 +1213,7 @@
       <c r="J5" s="3">
         <v>127</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>68</v>
       </c>
       <c r="L5" s="3">
@@ -892,19 +1228,19 @@
       <c r="O5">
         <v>86</v>
       </c>
-      <c r="Q5" s="17">
-        <v>66</v>
-      </c>
-      <c r="R5" s="11">
-        <f>Q5-L5</f>
-        <v>-32</v>
+      <c r="Q5" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" s="10">
+        <f t="shared" ref="R5:R19" si="0">L5-Q5</f>
+        <v>32</v>
       </c>
       <c r="S5" s="8">
-        <f>Q5-M5</f>
-        <v>-11.295274042005587</v>
+        <f t="shared" ref="S5:S19" si="1">M5-Q5</f>
+        <v>11.295274042005587</v>
       </c>
       <c r="T5" s="8">
-        <f>N5-Q5</f>
+        <f t="shared" ref="T5:T19" si="2">N5-Q5</f>
         <v>20</v>
       </c>
       <c r="W5">
@@ -948,7 +1284,7 @@
       <c r="J6" s="3">
         <v>23</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>26</v>
       </c>
       <c r="L6" s="3">
@@ -963,19 +1299,19 @@
       <c r="O6">
         <v>40</v>
       </c>
-      <c r="Q6" s="17">
-        <v>36</v>
-      </c>
-      <c r="R6" s="11">
-        <f>Q6-L6</f>
-        <v>-12</v>
+      <c r="Q6" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="R6" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="S6" s="8">
-        <f>Q6-M6</f>
-        <v>-1.3749472536413521</v>
+        <f t="shared" si="1"/>
+        <v>1.3749472536413521</v>
       </c>
       <c r="T6" s="8">
-        <f>N6-Q6</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="W6">
@@ -1034,10 +1370,21 @@
       <c r="O7">
         <v>30</v>
       </c>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
+      <c r="Q7" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="S7" s="8">
+        <f t="shared" si="1"/>
+        <v>1.2963396730067487</v>
+      </c>
+      <c r="T7" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="W7">
         <v>40</v>
       </c>
@@ -1094,10 +1441,21 @@
       <c r="O8">
         <v>30</v>
       </c>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+      <c r="Q8" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="R8" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.43119563915550074</v>
+      </c>
+      <c r="T8" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="W8">
         <v>30</v>
       </c>
@@ -1154,10 +1512,21 @@
       <c r="O9">
         <v>28</v>
       </c>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
+      <c r="Q9" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="R9" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.93465931102369026</v>
+      </c>
+      <c r="T9" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="W9">
         <v>30</v>
       </c>
@@ -1214,10 +1583,21 @@
       <c r="O10">
         <v>176</v>
       </c>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
+      <c r="Q10" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="R10" s="10">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="S10" s="8">
+        <f t="shared" si="1"/>
+        <v>27.996064717609897</v>
+      </c>
+      <c r="T10" s="8">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
       <c r="W10">
         <v>28</v>
       </c>
@@ -1275,7 +1655,7 @@
         <v>84</v>
       </c>
       <c r="Q11" s="15"/>
-      <c r="R11" s="11"/>
+      <c r="R11" s="10"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="W11">
@@ -1319,7 +1699,7 @@
       <c r="J12" s="3">
         <v>21</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="14">
         <v>38</v>
       </c>
       <c r="L12" s="3">
@@ -1334,19 +1714,19 @@
       <c r="O12">
         <v>72</v>
       </c>
-      <c r="Q12" s="17">
-        <v>48</v>
-      </c>
-      <c r="R12" s="11">
-        <f>Q12-L12</f>
-        <v>-20</v>
+      <c r="Q12" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="R12" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="S12" s="8">
-        <f>Q12-M12</f>
-        <v>-11.890885753675519</v>
+        <f t="shared" si="1"/>
+        <v>11.890885753675519</v>
       </c>
       <c r="T12" s="8">
-        <f>N12-Q12</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="W12">
@@ -1405,10 +1785,21 @@
       <c r="O13">
         <v>48</v>
       </c>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="Q13" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="R13" s="10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="S13" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.51334355238336116</v>
+      </c>
+      <c r="T13" s="8">
+        <f t="shared" si="2"/>
+        <v>-16</v>
+      </c>
       <c r="W13">
         <v>72</v>
       </c>
@@ -1450,7 +1841,7 @@
       <c r="J14" s="3">
         <v>15</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="14">
         <v>45</v>
       </c>
       <c r="L14" s="3">
@@ -1465,19 +1856,19 @@
       <c r="O14">
         <v>68</v>
       </c>
-      <c r="Q14" s="17">
-        <v>54</v>
-      </c>
-      <c r="R14" s="11">
-        <f>Q14-L14</f>
-        <v>-16</v>
+      <c r="Q14" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="S14" s="8">
-        <f>Q14-M14</f>
-        <v>-7.6177329147960791</v>
+        <f t="shared" si="1"/>
+        <v>7.6177329147960791</v>
       </c>
       <c r="T14" s="8">
-        <f>N14-Q14</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="W14">
@@ -1521,7 +1912,7 @@
       <c r="J15" s="3">
         <v>15</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="14">
         <v>81</v>
       </c>
       <c r="L15" s="3">
@@ -1536,19 +1927,19 @@
       <c r="O15">
         <v>40</v>
       </c>
-      <c r="Q15" s="17">
-        <v>76</v>
-      </c>
-      <c r="R15" s="11">
-        <f>Q15-L15</f>
-        <v>-38</v>
+      <c r="Q15" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="R15" s="10">
+        <f t="shared" si="0"/>
+        <v>38</v>
       </c>
       <c r="S15" s="8">
-        <f>Q15-M15</f>
-        <v>-60.220462732987812</v>
+        <f t="shared" si="1"/>
+        <v>60.220462732987812</v>
       </c>
       <c r="T15" s="8">
-        <f>N15-Q15</f>
+        <f t="shared" si="2"/>
         <v>-36</v>
       </c>
       <c r="W15">
@@ -1592,7 +1983,7 @@
       <c r="J16" s="3">
         <v>27</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="14">
         <v>424</v>
       </c>
       <c r="L16" s="3">
@@ -1607,19 +1998,19 @@
       <c r="O16">
         <v>340</v>
       </c>
-      <c r="Q16" s="17">
-        <v>414</v>
-      </c>
-      <c r="R16" s="11">
-        <f t="shared" ref="R16:R17" si="0">Q16-L16</f>
-        <v>-46</v>
+      <c r="Q16" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="S16" s="8">
-        <f t="shared" ref="S16:S17" si="1">Q16-M16</f>
-        <v>-48.144636599823627</v>
+        <f t="shared" si="1"/>
+        <v>48.144636599823627</v>
       </c>
       <c r="T16" s="8">
-        <f t="shared" ref="T16:T17" si="2">N16-Q16</f>
+        <f t="shared" si="2"/>
         <v>-74</v>
       </c>
       <c r="W16">
@@ -1628,7 +2019,7 @@
       <c r="X16">
         <v>235980</v>
       </c>
-      <c r="AB16" s="28">
+      <c r="AB16" s="24">
         <v>46</v>
       </c>
       <c r="AC16">
@@ -1666,7 +2057,7 @@
       <c r="J17" s="3">
         <v>21</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="14">
         <v>373</v>
       </c>
       <c r="L17" s="3">
@@ -1681,28 +2072,28 @@
       <c r="O17">
         <v>340</v>
       </c>
-      <c r="Q17" s="17">
-        <v>398</v>
-      </c>
-      <c r="R17" s="11">
+      <c r="Q17" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="R17" s="10">
         <f t="shared" si="0"/>
-        <v>-22</v>
+        <v>22</v>
       </c>
       <c r="S17" s="8">
         <f t="shared" si="1"/>
-        <v>-9.9055187250251038</v>
+        <v>9.9055187250251038</v>
       </c>
       <c r="T17" s="8">
         <f t="shared" si="2"/>
         <v>-58</v>
       </c>
-      <c r="W17" s="28">
+      <c r="W17" s="24">
         <v>46</v>
       </c>
-      <c r="X17" s="28">
+      <c r="X17" s="24">
         <v>235981</v>
       </c>
-      <c r="AB17" s="28">
+      <c r="AB17" s="24">
         <v>44</v>
       </c>
       <c r="AC17">
@@ -1756,13 +2147,13 @@
         <v>46</v>
       </c>
       <c r="Q18" s="15"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="W18" s="28">
+      <c r="R18" s="10"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="W18" s="24">
         <v>44</v>
       </c>
-      <c r="X18" s="28">
+      <c r="X18" s="24">
         <v>235984</v>
       </c>
       <c r="AC18">
@@ -1815,10 +2206,21 @@
       <c r="O19">
         <v>40</v>
       </c>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+      <c r="Q19" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="R19" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="S19" s="8">
+        <f t="shared" si="1"/>
+        <v>1.3802044943976668</v>
+      </c>
+      <c r="T19" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="W19">
         <v>340</v>
       </c>
@@ -1832,15 +2234,15 @@
       </c>
       <c r="R20">
         <f>SUMSQ(R3:R19)</f>
-        <v>5968</v>
+        <v>9985</v>
       </c>
       <c r="S20">
-        <f>SUMSQ(S4:S17)</f>
-        <v>6374.6316829500811</v>
+        <f>SUMSQ(S3:S19)</f>
+        <v>7163.3198229265336</v>
       </c>
       <c r="T20">
-        <f>SUMSQ(T4:T17)</f>
-        <v>11388</v>
+        <f>SUMSQ(T3:T19)</f>
+        <v>12684</v>
       </c>
       <c r="W20">
         <v>340</v>
@@ -1848,7 +2250,7 @@
       <c r="X20">
         <v>235986</v>
       </c>
-      <c r="AB20" s="28">
+      <c r="AB20" s="24">
         <v>46</v>
       </c>
     </row>
@@ -1857,21 +2259,21 @@
         <v>15</v>
       </c>
       <c r="R21">
-        <f>COUNT(Q3:Q19)</f>
-        <v>8</v>
+        <f>COUNT(R3:R19)</f>
+        <v>14</v>
       </c>
       <c r="S21">
-        <f>COUNT(R3:R19)</f>
-        <v>8</v>
+        <f>COUNT(S3:S19)</f>
+        <v>14</v>
       </c>
       <c r="T21">
-        <f>COUNT(S3:S19)</f>
-        <v>8</v>
-      </c>
-      <c r="W21" s="28">
+        <f>COUNT(T3:T19)</f>
+        <v>14</v>
+      </c>
+      <c r="W21" s="24">
         <v>46</v>
       </c>
-      <c r="X21" s="28">
+      <c r="X21" s="24">
         <v>235983</v>
       </c>
     </row>
@@ -1879,11 +2281,11 @@
       <c r="M22">
         <v>55.680476331125107</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="16">
         <v>44</v>
       </c>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
       <c r="W22">
         <v>46</v>
       </c>
@@ -1895,10 +2297,10 @@
       <c r="M23" s="3">
         <v>41.756478138640432</v>
       </c>
-      <c r="N23" s="21">
+      <c r="N23" s="17">
         <v>44</v>
       </c>
-      <c r="R23" s="12" t="s">
+      <c r="R23" s="11" t="s">
         <v>18</v>
       </c>
       <c r="S23" s="4" t="s">
@@ -1914,179 +2316,859 @@
         <v>236025</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="26" t="s">
+        <v>31</v>
+      </c>
       <c r="M24" s="3">
         <v>84.929670372295817</v>
       </c>
-      <c r="N24" s="21">
+      <c r="N24" s="17">
         <v>46</v>
       </c>
-      <c r="R24" s="13">
+      <c r="R24" s="12">
         <f>SQRT(R20/R21)</f>
-        <v>27.313000567495326</v>
+        <v>26.706072075733744</v>
       </c>
       <c r="S24" s="5">
         <f>SQRT(S20/S21)</f>
-        <v>28.228158997156726</v>
+        <v>22.620028771812152</v>
       </c>
       <c r="T24" s="5">
         <f>SQRT(T20/T21)</f>
-        <v>37.729298959826963</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+        <v>30.099833886584822</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="M25" s="3">
         <v>37.825875345796227</v>
       </c>
-      <c r="N25" s="21">
+      <c r="N25" s="17">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="M26">
         <v>35.751889036750981</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="16">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="26" t="s">
+        <v>24</v>
+      </c>
       <c r="M27">
         <v>34.905428976361989</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="16">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="M28">
         <v>33.078834354332727</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="16">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="26" t="s">
+        <v>26</v>
+      </c>
       <c r="M29">
         <v>173.98223948728511</v>
       </c>
-      <c r="N29" s="20">
+      <c r="N29" s="16">
         <v>296</v>
       </c>
-      <c r="R29" s="22" t="s">
+      <c r="R29" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="S29" s="23" t="s">
+      <c r="S29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="T29" s="23" t="s">
+      <c r="T29" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="M30">
         <v>91.539508452843435</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N30" s="16">
         <v>44</v>
       </c>
-      <c r="R30" s="24">
+      <c r="R30" s="20">
         <v>20.518284528683193</v>
       </c>
-      <c r="S30" s="25">
+      <c r="S30" s="21">
         <v>25.685944108302962</v>
       </c>
-      <c r="T30" s="25">
+      <c r="T30" s="21">
         <v>20.607442021431645</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="26" t="s">
+        <v>28</v>
+      </c>
       <c r="M31" s="3">
         <v>59.626571692041168</v>
       </c>
-      <c r="N31" s="21">
+      <c r="N31" s="17">
         <v>44</v>
       </c>
-      <c r="R31" s="26" t="s">
+      <c r="R31" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="S31" s="27" t="s">
+      <c r="S31" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="T31" s="27" t="s">
+      <c r="T31" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="M32">
         <v>67.174074696381723</v>
       </c>
-      <c r="N32" s="20">
+      <c r="N32" s="16">
         <v>44</v>
       </c>
-      <c r="R32" s="24">
+      <c r="R32" s="20">
         <v>27.313000567495326</v>
       </c>
-      <c r="S32" s="25">
+      <c r="S32" s="21">
         <v>26.901318448855392</v>
       </c>
-      <c r="T32" s="25">
+      <c r="T32" s="21">
         <v>66.075714146727165</v>
       </c>
     </row>
-    <row r="33" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33" s="26" t="s">
+        <v>30</v>
+      </c>
       <c r="M33" s="3">
         <v>64.088337109654304</v>
       </c>
-      <c r="N33" s="21">
+      <c r="N33" s="17">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="M34" s="3">
         <v>109.9056922983319</v>
       </c>
-      <c r="N34" s="21">
+      <c r="N34" s="17">
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M35" s="3">
         <v>473.38039538904297</v>
       </c>
-      <c r="N35" s="21">
+      <c r="N35" s="17">
         <v>340</v>
       </c>
     </row>
-    <row r="36" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="M36" s="3">
         <v>420.38506339881877</v>
       </c>
-      <c r="N36" s="21">
+      <c r="N36" s="17">
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="26" t="s">
+        <v>33</v>
+      </c>
       <c r="M37">
         <v>41.900994858328531</v>
       </c>
-      <c r="N37" s="20">
+      <c r="N37" s="16">
         <v>44</v>
       </c>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-    </row>
-    <row r="38" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="O37" s="16"/>
+    </row>
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="M38">
         <v>39.768322133434268</v>
       </c>
       <c r="N38" s="6">
         <v>44</v>
       </c>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
+      <c r="O38" s="25"/>
+    </row>
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B42" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>235832</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="35"/>
+    </row>
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B45" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>235876</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>235878</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>235880</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>235881</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>235883</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>235882</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>235798</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>235905</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="35"/>
+    </row>
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>235909</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>235964</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>235979</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>235980</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B58" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B59" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B60" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B61" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>235985</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>235986</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B64" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B65" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>236021</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="35"/>
+    </row>
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>236025</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="35" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D9E122-1582-304C-B0B2-343D0E019C37}">
+  <dimension ref="B1:C47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:3" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B14" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="26"/>
+    </row>
+    <row r="40" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B42" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B44" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B45" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B47" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>